<commit_message>
Weer een stuk verder
Bezig met tweede biologische deelvraag. Venndiagram is klaar
</commit_message>
<xml_diff>
--- a/Docs/StatusPlanning.xlsx
+++ b/Docs/StatusPlanning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Sebastiaan</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Bezig</t>
+  </si>
+  <si>
+    <t>Niet nodig</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>Zoek combinatie van motifs in het hele humane genoom</t>
   </si>
 </sst>
 </file>
@@ -445,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,20 +543,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:5" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -565,6 +574,21 @@
         <v>0</v>
       </c>
       <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>